<commit_message>
demos and slides finished
</commit_message>
<xml_diff>
--- a/SECTOR 2016 - G.Tool/demo/demo3c/vulnmgmt.xlsx
+++ b/SECTOR 2016 - G.Tool/demo/demo3c/vulnmgmt.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Vulnerability ID</t>
   </si>
@@ -29,6 +29,9 @@
     <t>Categorization</t>
   </si>
   <si>
+    <t>CVSSv2 Score</t>
+  </si>
+  <si>
     <t>CWE Score</t>
   </si>
   <si>
@@ -51,6 +54,9 @@
   </si>
   <si>
     <t>Patch</t>
+  </si>
+  <si>
+    <t>6.1</t>
   </si>
   <si>
     <t>12/21/2015</t>
@@ -460,13 +466,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,66 +485,72 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -548,13 +560,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,95 +579,98 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>